<commit_message>
update report 6 + test list
</commit_message>
<xml_diff>
--- a/test list.xlsx
+++ b/test list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator.MAYTINH-L3JT85N\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new place\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="60">
   <si>
     <t>No</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Appointment time ko select được từ 9h tối trở đi. Lúc chạy được mặc định là 8h30, lúc chạy ko được thì ko có mặc định, select cũng không được luôn.)</t>
+  </si>
+  <si>
+    <t>Generate AssignedShift</t>
+  </si>
+  <si>
+    <t>Xóa hết dữ liệu trong bảng, nhập liệu như thế nào để hệ thống biết cách tự genarate thêm</t>
   </si>
 </sst>
 </file>
@@ -427,8 +433,8 @@
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>447675</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>400050</xdr:rowOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1579,8 +1585,8 @@
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>447675</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>400050</xdr:rowOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2236,7 +2242,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2273,7 +2281,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -2291,7 +2299,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -2517,7 +2525,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -2545,7 +2553,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>18</v>
       </c>
@@ -2713,11 +2721,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="B32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="5">

</xml_diff>

<commit_message>
update code + test list
</commit_message>
<xml_diff>
--- a/test list.xlsx
+++ b/test list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="93">
   <si>
     <t>No</t>
   </si>
@@ -193,12 +193,6 @@
     <t>Nếu select all, rồi send request thì hiện pop-up thông báo Error! You have to select at least one IP Address --&gt; bỏ popup, tìm cách validate bằng annotation. Và select all thì vẫn send request được bình thường</t>
   </si>
   <si>
-    <t>View Detail Request Change IP</t>
-  </si>
-  <si>
-    <t>Khi tạo request return ip, chọn defaultip thì hệ thống sẽ tự động select all, rồi gửi send request. Lúc này hệ thống redirect đến trạng request detail, thì bảng ip return có dữ liệu dư thừa cuối bảng "on" --&gt; why???</t>
-  </si>
-  <si>
     <t>Appointment time ko select được từ 9h tối trở đi. Lúc chạy được mặc định là 8h30, lúc chạy ko được thì ko có mặc định, select cũng không được luôn.)</t>
   </si>
   <si>
@@ -236,6 +230,81 @@
   </si>
   <si>
     <t>Hiển thị những thông tin liên quan đến request như. Số lượng requests đến trong ngày. Số lượng request đã xử lý rồi, chưa,.. Những request mới nhất. Thêm mới khách hàng,… có cần hiển thị không?</t>
+  </si>
+  <si>
+    <t>Nếu là request của khách thì hình khác, thông báo task của staff thì hình khác</t>
+  </si>
+  <si>
+    <t>Assign Shift</t>
+  </si>
+  <si>
+    <t>Set ngày đầu tiên bằng hệ thống, do manager làm</t>
+  </si>
+  <si>
+    <t>View Detail Request Return IP</t>
+  </si>
+  <si>
+    <t>làm sao để thằng shifthead/staff ca sau biết được ca trước còn lại những request nào chưa xử lý hoặc đang xử lý dang dở --&gt; filter mặc định status pending, waiting và processing</t>
+  </si>
+  <si>
+    <t>Tạo request, rồi hẹn appointment time là ngày khác, để đến lúc đó mới bấm nút Process được</t>
+  </si>
+  <si>
+    <t>Required filed</t>
+  </si>
+  <si>
+    <t>Những field bắt buộc nhập vào sẽ hiện (*)</t>
+  </si>
+  <si>
+    <t>Ca kiếp</t>
+  </si>
+  <si>
+    <t>Làm sao để biết Group nào đang làm việc trong ca</t>
+  </si>
+  <si>
+    <t>Click vào sự kiện ở schedule thì hiện ra popup ko rõ ý nghĩa</t>
+  </si>
+  <si>
+    <t>Validate nếu không chọn assign ip và assign location thì sao</t>
+  </si>
+  <si>
+    <t>List of IP Address</t>
+  </si>
+  <si>
+    <t>Select default radio button</t>
+  </si>
+  <si>
+    <t>Tự động suggest appointment time để khách hàng khỏi chọn. Nếu nó chọn buổi tối thì tự động suggest sang buổi sáng</t>
+  </si>
+  <si>
+    <t>Validate serial number và partnumber chỉ được nhập vào số</t>
+  </si>
+  <si>
+    <t>Request offline</t>
+  </si>
+  <si>
+    <t>Lúc request đến thì assignee là [Not aSSIGNED] --&gt; hiện ra shifthead ở ca hiện tại</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiển thị location của server </t>
+  </si>
+  <si>
+    <t>Quy định hiển thị A1 U34. Chỉnh hết các trang đồng bộ</t>
+  </si>
+  <si>
+    <t>Description của request</t>
+  </si>
+  <si>
+    <t>Làm sao để lưu xuống hàng lúc nhập vào db</t>
+  </si>
+  <si>
+    <t>Number of Ips hiển thị dynamic chứ ko set cứng (cả 2 fields luôn)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process request </t>
+  </si>
+  <si>
+    <t>thằng thực thi mới thấy content, máy thằng còn lại chỉ thấy request của khách hàng</t>
   </si>
 </sst>
 </file>
@@ -265,12 +334,18 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -285,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -303,6 +378,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -354,7 +441,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1679,8 +1766,8 @@
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>438150</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>323850</xdr:rowOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1744,7 +1831,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>447675</xdr:colOff>
           <xdr:row>23</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1991,8 +2078,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G53" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A2:G53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:G71" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A2:G71"/>
   <tableColumns count="7">
     <tableColumn id="1" name="No" dataDxfId="6"/>
     <tableColumn id="2" name="Function" dataDxfId="5"/>
@@ -2270,10 +2357,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:G53"/>
+  <dimension ref="A2:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,23 +2398,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+    <row r="3" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="10"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -2337,60 +2424,62 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="5" spans="1:7" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" s="8" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="C7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
@@ -2439,7 +2528,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="F10" s="6"/>
     </row>
@@ -2472,7 +2561,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="F12" s="6"/>
     </row>
@@ -2528,21 +2617,23 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+    <row r="16" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="D16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>15</v>
       </c>
@@ -2556,7 +2647,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>16</v>
       </c>
@@ -2570,7 +2661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>17</v>
       </c>
@@ -2584,35 +2675,39 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+    <row r="20" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="D21" s="7"/>
+      <c r="E21" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>20</v>
       </c>
@@ -2623,10 +2718,10 @@
         <v>40</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>21</v>
       </c>
@@ -2637,24 +2732,26 @@
         <v>42</v>
       </c>
       <c r="E23" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>22</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>23</v>
       </c>
@@ -2668,7 +2765,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>24</v>
       </c>
@@ -2679,10 +2776,10 @@
         <v>47</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>25</v>
       </c>
@@ -2693,10 +2790,10 @@
         <v>50</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>26</v>
       </c>
@@ -2704,13 +2801,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -2724,88 +2821,99 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+    <row r="30" spans="1:6" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
         <v>28</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="D30" s="7"/>
+      <c r="E30" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="D31" s="7"/>
+      <c r="E31" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>30</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="C33" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>31</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -2813,27 +2921,27 @@
         <v>24</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -2841,13 +2949,13 @@
         <v>41</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -2855,95 +2963,339 @@
         <v>20</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+    <row r="40" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>38</v>
       </c>
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="B40" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <v>39</v>
       </c>
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="B41" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>40</v>
       </c>
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>41</v>
-      </c>
-      <c r="C43" s="3"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="B42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
         <v>42</v>
       </c>
-      <c r="C44" s="3"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>43</v>
-      </c>
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
         <v>44</v>
       </c>
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>45</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
-        <v>45</v>
-      </c>
-      <c r="C47" s="3"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
         <v>46</v>
       </c>
-      <c r="C48" s="3"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
+      <c r="B47" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
         <v>47</v>
       </c>
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>48</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
-        <v>48</v>
-      </c>
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
-        <v>49</v>
-      </c>
-      <c r="C51" s="3"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
-        <v>50</v>
-      </c>
-      <c r="C52" s="3"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
-        <v>51</v>
-      </c>
-      <c r="C53" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="C71" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3385,8 +3737,8 @@
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>438150</xdr:colOff>
-                    <xdr:row>21</xdr:row>
-                    <xdr:rowOff>323850</xdr:rowOff>
+                    <xdr:row>22</xdr:row>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -3408,7 +3760,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>447675</xdr:colOff>
                     <xdr:row>23</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
+                    <xdr:rowOff>47625</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
update class diagram + usecase + physical diagram 20160411
</commit_message>
<xml_diff>
--- a/test list.xlsx
+++ b/test list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="105">
   <si>
     <t>No</t>
   </si>
@@ -332,6 +332,15 @@
   </si>
   <si>
     <t>Default IP đang ko đc hiện lên</t>
+  </si>
+  <si>
+    <t>Server Index</t>
+  </si>
+  <si>
+    <t>Lỗi filter bảng list servers</t>
+  </si>
+  <si>
+    <t>liệt kê hết staff trong hệ thống ra --&gt; sửa lại trường hợp nó cho đổi ca trực</t>
   </si>
 </sst>
 </file>
@@ -2404,8 +2413,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3328,13 +3337,29 @@
       <c r="A61" s="5">
         <v>61</v>
       </c>
-      <c r="C61" s="3"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>62</v>
       </c>
-      <c r="C62" s="3"/>
+      <c r="B62" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="5">

</xml_diff>

<commit_message>
update delete add server + regex
</commit_message>
<xml_diff>
--- a/test list.xlsx
+++ b/test list.xlsx
@@ -446,13 +446,13 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -493,10 +493,10 @@
   </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" name="No" dataDxfId="4"/>
-    <tableColumn id="2" name="Function" dataDxfId="0"/>
-    <tableColumn id="3" name="Description" dataDxfId="3"/>
-    <tableColumn id="4" name="Assignee" dataDxfId="2"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
+    <tableColumn id="2" name="Function" dataDxfId="3"/>
+    <tableColumn id="3" name="Description" dataDxfId="2"/>
+    <tableColumn id="4" name="Assignee" dataDxfId="1"/>
+    <tableColumn id="5" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -768,8 +768,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +815,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update home, request page
</commit_message>
<xml_diff>
--- a/test list.xlsx
+++ b/test list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="125">
   <si>
     <t>No</t>
   </si>
@@ -374,6 +374,33 @@
   </si>
   <si>
     <t>Xem trang icon của adminlte</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Click vào pending, dẫn đến trang list request và tự search  request ở trạng thái pending hôm nay. Processing request cà this week request cũng vậy</t>
+  </si>
+  <si>
+    <t>Click vào Tab running server --&gt; dẫn đến trang list server sẽ tự filter là "Running"</t>
+  </si>
+  <si>
+    <t>List request</t>
+  </si>
+  <si>
+    <t>Mặc định mới vào sẽ chọn request today + pending&amp;Processing</t>
+  </si>
+  <si>
+    <t>Test Lại tất cả những trường hợp có thể chạy real time</t>
+  </si>
+  <si>
+    <t>List customer request</t>
+  </si>
+  <si>
+    <t>Bổ sung status pending &amp; processing</t>
+  </si>
+  <si>
+    <t>set mặc định là pending&amp;processing</t>
   </si>
 </sst>
 </file>
@@ -429,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -467,16 +494,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -513,8 +543,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F69" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A2:F69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:F73" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A2:F73">
     <filterColumn colId="4">
       <filters>
         <filter val="Pending"/>
@@ -526,8 +556,8 @@
     <tableColumn id="2" name="Function" dataDxfId="4"/>
     <tableColumn id="3" name="Description" dataDxfId="3"/>
     <tableColumn id="4" name="Assignee" dataDxfId="2"/>
-    <tableColumn id="5" name="Status" dataDxfId="1"/>
-    <tableColumn id="6" name="Column1" dataDxfId="0"/>
+    <tableColumn id="5" name="Status" dataDxfId="0"/>
+    <tableColumn id="6" name="Column1" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -797,10 +827,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:F72"/>
+  <dimension ref="A2:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -884,7 +914,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="10" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="10" customFormat="1" ht="34.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -896,13 +926,13 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="10" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" s="10" customFormat="1" ht="54" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -914,7 +944,7 @@
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>111</v>
@@ -1181,18 +1211,18 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" s="7" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
+    <row r="24" spans="1:6" s="3" customFormat="1" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
         <v>22</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6" t="s">
+      <c r="D24" s="13"/>
+      <c r="E24" s="13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1271,48 +1301,45 @@
       </c>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" s="7" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+    <row r="30" spans="1:6" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>28</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" s="7" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+      <c r="E30" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>29</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="7" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6">
+      <c r="E31" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="13" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1424,7 +1451,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="7" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="7" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>39</v>
       </c>
@@ -1483,7 +1510,7 @@
         <v>70</v>
       </c>
       <c r="D43" s="2"/>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="5" t="s">
         <v>46</v>
       </c>
       <c r="F43" s="2"/>
@@ -1548,20 +1575,20 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
+    <row r="48" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
         <v>49</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="2"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -1608,20 +1635,20 @@
       </c>
       <c r="F51" s="2"/>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
+    <row r="52" spans="1:6" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
         <v>53</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E52" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="2"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="53" spans="1:6" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="9">
@@ -1818,36 +1845,112 @@
       </c>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>67</v>
       </c>
-      <c r="C66" s="3"/>
+      <c r="B66" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F66" s="2"/>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>68</v>
       </c>
-      <c r="C67" s="3"/>
+      <c r="B67" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F67" s="2"/>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>69</v>
       </c>
-      <c r="C68" s="3"/>
+      <c r="B68" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>70</v>
       </c>
-      <c r="C69" s="3"/>
+      <c r="B69" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="F69" s="2"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
+    <row r="70" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>71</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>72</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>73</v>
+      </c>
+      <c r="C72" s="3"/>
+      <c r="F72" s="2"/>
+    </row>
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>74</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="F73" s="2"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update icon of Notification and test list
</commit_message>
<xml_diff>
--- a/test list.xlsx
+++ b/test list.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\new place\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tien Huynh\Desktop\Data\GitHub_20012016\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -412,7 +412,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -850,8 +850,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,7 +1390,7 @@
         <v>58</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F34" s="2"/>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="9" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F39" s="10" t="s">
         <v>115</v>

</xml_diff>